<commit_message>
Created Success Page, Excel updation, vectors
</commit_message>
<xml_diff>
--- a/server/main.xlsx
+++ b/server/main.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1727,9 +1727,274 @@
         <v>Verification in progress...</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>1/1/2025</v>
+      </c>
+      <c r="B26" t="str">
+        <v>1:11:58 pm</v>
+      </c>
+      <c r="C26" t="str">
+        <v>010125131158</v>
+      </c>
+      <c r="D26" t="str">
+        <v>order_Pe6HZcMA3jtKOF</v>
+      </c>
+      <c r="E26" t="str">
+        <v>21</v>
+      </c>
+      <c r="F26" t="str">
+        <v>21B81A05V9</v>
+      </c>
+      <c r="G26" t="str">
+        <v>SAMRATH REDDY</v>
+      </c>
+      <c r="H26" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="I26" t="str">
+        <v>E</v>
+      </c>
+      <c r="J26" t="str">
+        <v>+917999999990</v>
+      </c>
+      <c r="K26" t="str">
+        <v>fomowog893@nozamas.com</v>
+      </c>
+      <c r="L26" t="str">
+        <v>CollegeFee</v>
+      </c>
+      <c r="M26" t="str">
+        <v>I</v>
+      </c>
+      <c r="N26" t="str">
+        <v/>
+      </c>
+      <c r="O26">
+        <v>120000</v>
+      </c>
+      <c r="P26" t="str">
+        <v>wallet</v>
+      </c>
+      <c r="Q26" t="str">
+        <v>Verification in progress...</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>1/1/2025</v>
+      </c>
+      <c r="B27" t="str">
+        <v>1:15:15 pm</v>
+      </c>
+      <c r="C27" t="str">
+        <v>010125131515</v>
+      </c>
+      <c r="D27" t="str">
+        <v>order_Pe6KAtrGxllVGc</v>
+      </c>
+      <c r="E27" t="str">
+        <v>21</v>
+      </c>
+      <c r="F27" t="str">
+        <v>21B81A05V9</v>
+      </c>
+      <c r="G27" t="str">
+        <v>SAMRATH REDDY</v>
+      </c>
+      <c r="H27" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="I27" t="str">
+        <v>E</v>
+      </c>
+      <c r="J27" t="str">
+        <v>+917999999990</v>
+      </c>
+      <c r="K27" t="str">
+        <v>fomowog893@nozamas.com</v>
+      </c>
+      <c r="L27" t="str">
+        <v>CollegeFee</v>
+      </c>
+      <c r="M27" t="str">
+        <v>I</v>
+      </c>
+      <c r="N27" t="str">
+        <v/>
+      </c>
+      <c r="O27">
+        <v>120000</v>
+      </c>
+      <c r="P27" t="str">
+        <v>wallet</v>
+      </c>
+      <c r="Q27" t="str">
+        <v>Verification in progress...</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>1/1/2025</v>
+      </c>
+      <c r="B28" t="str">
+        <v>3:10:43 pm</v>
+      </c>
+      <c r="C28" t="str">
+        <v>010125151043</v>
+      </c>
+      <c r="D28" t="str">
+        <v>order_Pe8IxBmB7VvSbS</v>
+      </c>
+      <c r="E28" t="str">
+        <v>21</v>
+      </c>
+      <c r="F28" t="str">
+        <v>21B81A05V9</v>
+      </c>
+      <c r="G28" t="str">
+        <v>SAMRATH REDDY</v>
+      </c>
+      <c r="H28" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="I28" t="str">
+        <v>E</v>
+      </c>
+      <c r="J28" t="str">
+        <v>+917981455290</v>
+      </c>
+      <c r="K28" t="str">
+        <v>samrathreddy04@gmail.com</v>
+      </c>
+      <c r="L28" t="str">
+        <v>CollegeFee</v>
+      </c>
+      <c r="M28" t="str">
+        <v>IV</v>
+      </c>
+      <c r="N28" t="str">
+        <v/>
+      </c>
+      <c r="O28">
+        <v>120000</v>
+      </c>
+      <c r="P28" t="str">
+        <v>wallet</v>
+      </c>
+      <c r="Q28" t="str">
+        <v>Verification in progress...</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>1/1/2025</v>
+      </c>
+      <c r="B29" t="str">
+        <v>3:30:19 pm</v>
+      </c>
+      <c r="C29" t="str">
+        <v>010125153019</v>
+      </c>
+      <c r="D29" t="str">
+        <v>order_Pe8dccfdSEBR2X</v>
+      </c>
+      <c r="E29" t="str">
+        <v>21</v>
+      </c>
+      <c r="F29" t="str">
+        <v>21B81A05V9</v>
+      </c>
+      <c r="G29" t="str">
+        <v>SAMRATH REDDY</v>
+      </c>
+      <c r="H29" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="I29" t="str">
+        <v>E</v>
+      </c>
+      <c r="J29" t="str">
+        <v>+917981455290</v>
+      </c>
+      <c r="K29" t="str">
+        <v>samrathreddy04@gmail.com</v>
+      </c>
+      <c r="L29" t="str">
+        <v>CollegeFee</v>
+      </c>
+      <c r="M29" t="str">
+        <v>IV</v>
+      </c>
+      <c r="N29" t="str">
+        <v/>
+      </c>
+      <c r="O29">
+        <v>120000</v>
+      </c>
+      <c r="P29" t="str">
+        <v>wallet</v>
+      </c>
+      <c r="Q29" t="str">
+        <v>Rejected</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>1/1/2025</v>
+      </c>
+      <c r="B30" t="str">
+        <v>3:35:52 pm</v>
+      </c>
+      <c r="C30" t="str">
+        <v>010125153552</v>
+      </c>
+      <c r="D30" t="str">
+        <v>order_Pe8jN3nSLdJf6t</v>
+      </c>
+      <c r="E30" t="str">
+        <v>21</v>
+      </c>
+      <c r="F30" t="str">
+        <v>21B81A05V9</v>
+      </c>
+      <c r="G30" t="str">
+        <v>SAMRATH REDDY</v>
+      </c>
+      <c r="H30" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="I30" t="str">
+        <v>E</v>
+      </c>
+      <c r="J30" t="str">
+        <v>+917981455290</v>
+      </c>
+      <c r="K30" t="str">
+        <v>samrathreddy04@gmail.com</v>
+      </c>
+      <c r="L30" t="str">
+        <v>CollegeFee</v>
+      </c>
+      <c r="M30" t="str">
+        <v>I</v>
+      </c>
+      <c r="N30" t="str">
+        <v/>
+      </c>
+      <c r="O30">
+        <v>120000</v>
+      </c>
+      <c r="P30" t="str">
+        <v>wallet</v>
+      </c>
+      <c r="Q30" t="str">
+        <v>Verified</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q30"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed success page GET issue(Hosting)
</commit_message>
<xml_diff>
--- a/server/main.xlsx
+++ b/server/main.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1992,9 +1992,168 @@
         <v>Verified</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>1/1/2025</v>
+      </c>
+      <c r="B31" t="str">
+        <v>4:57:58 pm</v>
+      </c>
+      <c r="C31" t="str">
+        <v>010125165758</v>
+      </c>
+      <c r="D31" t="str">
+        <v>order_PeA8Jf1J1MAb0G</v>
+      </c>
+      <c r="E31" t="str">
+        <v>21</v>
+      </c>
+      <c r="F31" t="str">
+        <v>21B81A05V9</v>
+      </c>
+      <c r="G31" t="str">
+        <v>SAMRATH REDDY</v>
+      </c>
+      <c r="H31" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="I31" t="str">
+        <v>E</v>
+      </c>
+      <c r="J31" t="str">
+        <v>+917981455290</v>
+      </c>
+      <c r="K31" t="str">
+        <v>samrathreddy04@gmail.com</v>
+      </c>
+      <c r="L31" t="str">
+        <v>CollegeFee</v>
+      </c>
+      <c r="M31" t="str">
+        <v>IV</v>
+      </c>
+      <c r="N31" t="str">
+        <v/>
+      </c>
+      <c r="O31">
+        <v>120000</v>
+      </c>
+      <c r="P31" t="str">
+        <v>wallet</v>
+      </c>
+      <c r="Q31" t="str">
+        <v>Verification in progress...</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>1/1/2025</v>
+      </c>
+      <c r="B32" t="str">
+        <v>5:27:06 pm</v>
+      </c>
+      <c r="C32" t="str">
+        <v>010125172706</v>
+      </c>
+      <c r="D32" t="str">
+        <v>order_PeAd37PCqw6j8f</v>
+      </c>
+      <c r="E32" t="str">
+        <v>21</v>
+      </c>
+      <c r="F32" t="str">
+        <v>21B81A05V9</v>
+      </c>
+      <c r="G32" t="str">
+        <v>SAMRATH REDDY</v>
+      </c>
+      <c r="H32" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="I32" t="str">
+        <v>E</v>
+      </c>
+      <c r="J32" t="str">
+        <v>+917981455290</v>
+      </c>
+      <c r="K32" t="str">
+        <v>samrathreddy04@gmail.com</v>
+      </c>
+      <c r="L32" t="str">
+        <v>CollegeFee</v>
+      </c>
+      <c r="M32" t="str">
+        <v>IV</v>
+      </c>
+      <c r="N32" t="str">
+        <v/>
+      </c>
+      <c r="O32">
+        <v>120000</v>
+      </c>
+      <c r="P32" t="str">
+        <v>wallet</v>
+      </c>
+      <c r="Q32" t="str">
+        <v>Verification in progress...</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>1/1/2025</v>
+      </c>
+      <c r="B33" t="str">
+        <v>5:29:27 pm</v>
+      </c>
+      <c r="C33" t="str">
+        <v>010125172927</v>
+      </c>
+      <c r="D33" t="str">
+        <v>order_PeAfX0B2PHevt5</v>
+      </c>
+      <c r="E33" t="str">
+        <v>21</v>
+      </c>
+      <c r="F33" t="str">
+        <v>21B81A05V9</v>
+      </c>
+      <c r="G33" t="str">
+        <v>SAMRATH REDDY</v>
+      </c>
+      <c r="H33" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="I33" t="str">
+        <v>E</v>
+      </c>
+      <c r="J33" t="str">
+        <v>+917981455290</v>
+      </c>
+      <c r="K33" t="str">
+        <v>samrathreddy04@gmail.com</v>
+      </c>
+      <c r="L33" t="str">
+        <v>CollegeFee</v>
+      </c>
+      <c r="M33" t="str">
+        <v>I</v>
+      </c>
+      <c r="N33" t="str">
+        <v/>
+      </c>
+      <c r="O33">
+        <v>120000</v>
+      </c>
+      <c r="P33" t="str">
+        <v>wallet</v>
+      </c>
+      <c r="Q33" t="str">
+        <v>Rejected</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q30"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q33"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed success page GET issue page(Hosting)
</commit_message>
<xml_diff>
--- a/server/main.xlsx
+++ b/server/main.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2151,9 +2151,62 @@
         <v>Rejected</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>1/1/2025</v>
+      </c>
+      <c r="B34" t="str">
+        <v>5:38:29 pm</v>
+      </c>
+      <c r="C34" t="str">
+        <v>010125173829</v>
+      </c>
+      <c r="D34" t="str">
+        <v>order_PeAp7aj0j7sjOl</v>
+      </c>
+      <c r="E34" t="str">
+        <v>21</v>
+      </c>
+      <c r="F34" t="str">
+        <v>21B81A05V9</v>
+      </c>
+      <c r="G34" t="str">
+        <v>SAMRATH REDDY</v>
+      </c>
+      <c r="H34" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="I34" t="str">
+        <v>E</v>
+      </c>
+      <c r="J34" t="str">
+        <v>+917981455290</v>
+      </c>
+      <c r="K34" t="str">
+        <v>samrathreddy04@gmail.com</v>
+      </c>
+      <c r="L34" t="str">
+        <v>CollegeFee</v>
+      </c>
+      <c r="M34" t="str">
+        <v>IV</v>
+      </c>
+      <c r="N34" t="str">
+        <v/>
+      </c>
+      <c r="O34">
+        <v>120000</v>
+      </c>
+      <c r="P34" t="str">
+        <v>wallet</v>
+      </c>
+      <c r="Q34" t="str">
+        <v>Verification in progress...</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q33"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q34"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>